<commit_message>
- Minor changes to word/excel templates - Fix: Added round in katastash_plhrwmhs amounts
</commit_message>
<xml_diff>
--- a/metakinhseis/templates/excel/tmpl_katastash_plhrwmhs.xlsx
+++ b/metakinhseis/templates/excel/tmpl_katastash_plhrwmhs.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29127"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4578B4EC-AD42-4E2A-9BCD-38CF16E79EA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BCF5190-C1D4-4579-B922-CEA9F9E2CA00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="20370" windowHeight="13185" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1905" yWindow="2325" windowWidth="25050" windowHeight="12270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Φύλλο1" sheetId="1" r:id="rId1"/>
@@ -616,17 +616,17 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Κανονικό" xfId="0" builtinId="0"/>
@@ -990,8 +990,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A3:V26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="L23" sqref="L23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1006,6 +1006,7 @@
     <col min="9" max="9" width="6.7109375" customWidth="1"/>
     <col min="10" max="10" width="5.42578125" customWidth="1"/>
     <col min="11" max="11" width="8.7109375" customWidth="1"/>
+    <col min="14" max="14" width="11.42578125" customWidth="1"/>
     <col min="17" max="17" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1026,10 +1027,10 @@
       <c r="N3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="O3" s="39" t="s">
+      <c r="O3" s="45" t="s">
         <v>43</v>
       </c>
-      <c r="P3" s="39"/>
+      <c r="P3" s="45"/>
       <c r="Q3" s="16"/>
     </row>
     <row r="4" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
@@ -1051,10 +1052,10 @@
       <c r="N4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="O4" s="39" t="s">
+      <c r="O4" s="45" t="s">
         <v>44</v>
       </c>
-      <c r="P4" s="39"/>
+      <c r="P4" s="45"/>
       <c r="Q4" s="16"/>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
@@ -1069,15 +1070,15 @@
         <v>2</v>
       </c>
       <c r="G5" s="1"/>
-      <c r="H5" s="42" t="s">
+      <c r="H5" s="39" t="s">
         <v>46</v>
       </c>
-      <c r="I5" s="45"/>
-      <c r="J5" s="45"/>
-      <c r="K5" s="45"/>
-      <c r="L5" s="45"/>
+      <c r="I5" s="44"/>
+      <c r="J5" s="44"/>
+      <c r="K5" s="44"/>
+      <c r="L5" s="44"/>
       <c r="M5" s="1"/>
-      <c r="N5" s="41" t="s">
+      <c r="N5" s="43" t="s">
         <v>45</v>
       </c>
       <c r="O5" s="40"/>
@@ -1096,26 +1097,26 @@
       <c r="F6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G6" s="41" t="s">
+      <c r="G6" s="43" t="s">
         <v>40</v>
       </c>
-      <c r="H6" s="41"/>
+      <c r="H6" s="43"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="K6" s="41" t="s">
+      <c r="K6" s="43" t="s">
         <v>36</v>
       </c>
-      <c r="L6" s="41"/>
+      <c r="L6" s="43"/>
       <c r="M6" s="1"/>
       <c r="N6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="O6" s="39" t="s">
+      <c r="O6" s="45" t="s">
         <v>37</v>
       </c>
-      <c r="P6" s="39"/>
+      <c r="P6" s="45"/>
       <c r="Q6" s="16"/>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
@@ -1123,15 +1124,15 @@
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
-      <c r="F7" s="41" t="s">
+      <c r="F7" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="G7" s="41"/>
-      <c r="H7" s="41"/>
-      <c r="I7" s="41"/>
-      <c r="J7" s="41"/>
-      <c r="K7" s="41"/>
-      <c r="L7" s="41"/>
+      <c r="G7" s="43"/>
+      <c r="H7" s="43"/>
+      <c r="I7" s="43"/>
+      <c r="J7" s="43"/>
+      <c r="K7" s="43"/>
+      <c r="L7" s="43"/>
       <c r="M7" s="1"/>
       <c r="N7" s="1" t="s">
         <v>35</v>
@@ -1353,7 +1354,7 @@
       <c r="P14" s="20"/>
       <c r="Q14" s="20"/>
     </row>
-    <row r="15" spans="1:22" ht="62.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:22" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="35"/>
       <c r="B15" s="23"/>
       <c r="C15" s="37"/>
@@ -1456,10 +1457,10 @@
       <c r="Q17" s="10"/>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A18" s="44" t="s">
+      <c r="A18" s="42" t="s">
         <v>58</v>
       </c>
-      <c r="B18" s="44"/>
+      <c r="B18" s="42"/>
       <c r="C18" s="1"/>
       <c r="D18" s="9"/>
       <c r="E18" s="10"/>
@@ -1479,10 +1480,10 @@
       <c r="Q18" s="11"/>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A19" s="43" t="s">
+      <c r="A19" s="41" t="s">
         <v>34</v>
       </c>
-      <c r="B19" s="43"/>
+      <c r="B19" s="41"/>
       <c r="C19" s="1"/>
       <c r="D19" s="9"/>
       <c r="E19" s="10"/>
@@ -1551,7 +1552,7 @@
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
       <c r="K22" s="2"/>
-      <c r="L22" s="42" t="s">
+      <c r="L22" s="39" t="s">
         <v>59</v>
       </c>
       <c r="M22" s="40"/>
@@ -1619,6 +1620,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="O3:P3"/>
+    <mergeCell ref="O4:P4"/>
+    <mergeCell ref="O6:P6"/>
+    <mergeCell ref="P7:Q7"/>
+    <mergeCell ref="N5:Q5"/>
     <mergeCell ref="L22:N22"/>
     <mergeCell ref="A19:B19"/>
     <mergeCell ref="A18:B18"/>
@@ -1626,11 +1632,6 @@
     <mergeCell ref="H5:L5"/>
     <mergeCell ref="G6:H6"/>
     <mergeCell ref="F7:L7"/>
-    <mergeCell ref="O3:P3"/>
-    <mergeCell ref="O4:P4"/>
-    <mergeCell ref="O6:P6"/>
-    <mergeCell ref="P7:Q7"/>
-    <mergeCell ref="N5:Q5"/>
   </mergeCells>
   <pageMargins left="0.31496062992125984" right="0" top="0.35433070866141736" bottom="0.19685039370078741" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="75" orientation="landscape" r:id="rId1"/>

</xml_diff>